<commit_message>
ScrumLog Bjorn Jorissen 11/02/
</commit_message>
<xml_diff>
--- a/ScrumLogAppDev04.xlsx
+++ b/ScrumLogAppDev04.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenny\Desktop\ProjectAppDev04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11301497\Documents\GitHub\ProjectAppDev04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -253,9 +253,6 @@
     <t>Arne De Greef</t>
   </si>
   <si>
-    <t>Netwerkplan opstellen</t>
-  </si>
-  <si>
     <t>Gert Thora</t>
   </si>
   <si>
@@ -2392,13 +2389,16 @@
     <t>aan zijn piet getrokken</t>
   </si>
   <si>
-    <t>kruiswix met kevin</t>
-  </si>
-  <si>
     <t>Opmaken van use case diagram</t>
   </si>
   <si>
     <t>Verzamelen van info en documenten ter voorbereiding voor het project</t>
+  </si>
+  <si>
+    <t>Informatie verzamelen voor de analyse en vragen stellen aan de klant + analyse maken</t>
+  </si>
+  <si>
+    <t>Planning opstellen + helpen met het use case diagram</t>
   </si>
 </sst>
 </file>
@@ -2493,78 +2493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2577,11 +2509,11 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="191919"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -2617,7 +2549,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2689,7 +2621,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2841,7 +2773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -2884,19 +2816,19 @@
         <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2904,39 +2836,39 @@
         <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>790</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2949,7 +2881,7 @@
     </row>
     <row r="7" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -2960,79 +2892,79 @@
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="E8" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3045,7 +2977,7 @@
     </row>
     <row r="13" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3056,79 +2988,79 @@
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>362</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3196,112 +3128,112 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>449</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>455</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3317,7 +3249,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3331,115 +3263,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>582</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>591</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>716</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>719</v>
-      </c>
       <c r="E11" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>722</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3455,7 +3387,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3469,115 +3401,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>757</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>765</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>771</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>775</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>781</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>782</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>783</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>784</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3651,115 +3583,115 @@
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3775,7 +3707,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3789,115 +3721,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="G8" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>504</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3913,7 +3845,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3927,115 +3859,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>608</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>613</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>631</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>647</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>652</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>653</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>658</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>697</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>707</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,112 +4044,112 @@
         <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4233,7 +4165,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -4247,115 +4179,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>341</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>394</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>399</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4371,7 +4303,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -4385,115 +4317,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>517</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4570,112 +4502,112 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>339</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4691,7 +4623,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -4705,115 +4637,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>408</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>540</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>619</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4829,7 +4761,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -4843,115 +4775,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>644</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>661</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>665</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>675</v>
-      </c>
       <c r="H17" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>678</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5115,25 +5047,25 @@
         <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>167</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5149,7 +5081,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -5163,115 +5095,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5287,7 +5219,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -5301,115 +5233,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>551</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>677</v>
-      </c>
       <c r="E17" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>682</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>688</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5573,25 +5505,25 @@
         <v>61</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5607,7 +5539,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -5621,115 +5553,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>349</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>356</v>
-      </c>
       <c r="H11" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5745,7 +5677,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -5759,115 +5691,115 @@
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>378</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>383</v>
-      </c>
       <c r="I14" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>496</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>508</v>
-      </c>
       <c r="I17" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5941,115 +5873,115 @@
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>373</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>481</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>570</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>576</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>586</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>669</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6065,7 +5997,7 @@
     </row>
     <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -6079,115 +6011,115 @@
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>703</v>
-      </c>
       <c r="H8" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>705</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>729</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>734</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>746</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>747</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ScrumLog Kenny Vanrusselt 11/02/2015 final
</commit_message>
<xml_diff>
--- a/ScrumLogAppDev04.xlsx
+++ b/ScrumLogAppDev04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT 1 Week 1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Verzamelen van info en documenten ter voorbereiding voor het project</t>
-  </si>
-  <si>
     <t>Informatie verzamelen voor de analyse en vragen stellen aan de klant + analyse maken</t>
   </si>
   <si>
@@ -81,10 +78,13 @@
     <t>Gegevens over het project verzamelen als voorbereiding</t>
   </si>
   <si>
-    <t>Opmaken van use case diagram + omschrijving</t>
-  </si>
-  <si>
     <t>wa ik ga doen: helpen met use case diagram + wireframes opstellen</t>
+  </si>
+  <si>
+    <t>Verzamelen van info, Opmaken van use case diagram + omschrijving</t>
+  </si>
+  <si>
+    <t>Ontwerpen van mockups / layout</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -570,19 +570,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -590,19 +590,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Wat ik ga doen geremoved... cause kevin couldn't handle it
</commit_message>
<xml_diff>
--- a/ScrumLogAppDev04.xlsx
+++ b/ScrumLogAppDev04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT 1 Week 1" sheetId="1" r:id="rId1"/>
@@ -78,13 +78,13 @@
     <t>Gegevens over het project verzamelen als voorbereiding</t>
   </si>
   <si>
-    <t>wa ik ga doen: helpen met use case diagram + wireframes opstellen</t>
-  </si>
-  <si>
     <t>Verzamelen van info, Opmaken van use case diagram + omschrijving</t>
   </si>
   <si>
     <t>Ontwerpen van mockups / layout</t>
+  </si>
+  <si>
+    <t>helpen met use case diagram + wireframes opstellen</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -590,13 +590,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>

</xml_diff>